<commit_message>
Updated gitignore, ignore other changes
</commit_message>
<xml_diff>
--- a/generatortests/pw_test/T1/eq1.xlsx
+++ b/generatortests/pw_test/T1/eq1.xlsx
@@ -447,11 +447,11 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Bacteroides_cellulosilyticus</t>
+          <t>'Bacteroides_cellulosilyticus_DSM_14838.mat'</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.002597027565027085</v>
+        <v>0.016</v>
       </c>
     </row>
     <row r="3">
@@ -460,11 +460,11 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Bacteroides_coprocola</t>
+          <t>'Bacteroides_coprocola_M16_DSM_17136.mat'</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.01208409515296149</v>
+        <v>0.003</v>
       </c>
     </row>
     <row r="4">
@@ -473,11 +473,11 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Bacteroides_coprophilus</t>
+          <t>'Bacteroides_coprophilus_DSM_18228.mat'</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.001214801499682834</v>
+        <v>0.047</v>
       </c>
     </row>
     <row r="5">
@@ -486,11 +486,11 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Bacteroides_fluxus</t>
+          <t>'Bacteroides_fluxus_YIT_12057.mat'</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.001462369219837215</v>
+        <v>0.065</v>
       </c>
     </row>
     <row r="6">
@@ -499,11 +499,11 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Bacteroides_oleiciplenus</t>
+          <t>'Bacteroides_oleiciplenus_YIT_12058.mat'</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.01636250663127822</v>
+        <v>0.013</v>
       </c>
     </row>
     <row r="7">
@@ -512,11 +512,11 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Bacteroides_ovatus</t>
+          <t>'Bacteroides_ovatus_ATCC_8483.mat'</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.001918893180855844</v>
+        <v>0.23</v>
       </c>
     </row>
     <row r="8">
@@ -525,11 +525,11 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Bacteroides_plebeius</t>
+          <t>'Bacteroides_plebeius_M12_DSM_17135.mat'</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.00111032337925071</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -538,11 +538,11 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Bacteroides_salyersiae</t>
+          <t>'Bacteroides_salyersiae_WAL_10018.mat'</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0.01566360640950556</v>
+        <v>0.305</v>
       </c>
     </row>
     <row r="10">
@@ -551,11 +551,11 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Bacteroides_stercoris</t>
+          <t>'Bacteroides_stercoris_ATCC_43183.mat'</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0.003137588275088944</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
@@ -564,11 +564,11 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Bacteroides_thetaiotaomicron</t>
+          <t>'Bacteroides_thetaiotaomicron_VPI_5482.mat'</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.3179158886237279</v>
+        <v>-0</v>
       </c>
     </row>
     <row r="12">
@@ -577,11 +577,11 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Bacteroides_uniformis</t>
+          <t>'Bacteroides_uniformis_ATCC_8492.mat'</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0.001560682482231419</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
@@ -590,11 +590,11 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Bacteroides_vulgatus</t>
+          <t>'Bacteroides_vulgatus_ATCC_8482.mat'</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>0.1955707117328605</v>
+        <v>0.322</v>
       </c>
     </row>
     <row r="14">
@@ -603,11 +603,11 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Bifidobacterium_animalis</t>
+          <t>'Bifidobacterium_animalis_lactis_AD011.mat'</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>0.0199949058804634</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15">
@@ -616,11 +616,11 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Enterococcus_faecalis</t>
+          <t>'Enterococcus_faecalis_OG1RF_ATCC_47077.mat'</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>0.003581782520031733</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16">
@@ -629,11 +629,11 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Flavonifractor_plautii</t>
+          <t>'Flavonifractor_plautii_ATCC_29863.mat'</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>0.02804166795101209</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17">
@@ -642,11 +642,11 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Lactobacillus_plantarum</t>
+          <t>'Lactobacillus_plantarum_JDM1.mat'</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>0.001494815841089428</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18">
@@ -655,11 +655,11 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Odoribacter_laneus</t>
+          <t>'Odoribacter_laneus_YIT_12061.mat'</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>0.002253417845966155</v>
+        <v>-0</v>
       </c>
     </row>
     <row r="19">
@@ -668,11 +668,11 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Parabacteroides_distasonis</t>
+          <t>'Parabacteroides_distasonis_ATCC_8503.mat'</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>0.2603026945296619</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20">
@@ -681,11 +681,11 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Parabacteroides_johnsonii</t>
+          <t>'Parabacteroides_johnsonii_DSM_18315.mat'</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>0.002329342939696332</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>